<commit_message>
95. Unique Binary Search Trees II zen-30
</commit_message>
<xml_diff>
--- a/meta/progress.xlsx
+++ b/meta/progress.xlsx
@@ -1026,7 +1026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J104" sqref="J104"/>
+      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2647,7 +2647,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30">
+    <row r="96" spans="1:5" ht="30" hidden="1">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>5</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" hidden="1">
@@ -4106,7 +4106,7 @@
       </filters>
     </filterColumn>
     <filterColumn colId="1">
-      <filters blank="1">
+      <filters>
         <filter val="N"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Solution for "95. Unique Binary Search Trees II".
</commit_message>
<xml_diff>
--- a/meta/progress.xlsx
+++ b/meta/progress.xlsx
@@ -1026,7 +1026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J104" sqref="J104"/>
+      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2647,7 +2647,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30">
+    <row r="96" spans="1:5" ht="30" hidden="1">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>5</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" hidden="1">
@@ -4106,7 +4106,7 @@
       </filters>
     </filterColumn>
     <filterColumn colId="1">
-      <filters blank="1">
+      <filters>
         <filter val="N"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Solution for "81. Search in Rotated Sorted Array I & II". zen-1
</commit_message>
<xml_diff>
--- a/meta/progress.xlsx
+++ b/meta/progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="60" windowWidth="22960" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="14900" yWindow="860" windowWidth="22960" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2071,7 +2071,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" hidden="1">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" hidden="1">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>5</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30">
@@ -2698,7 +2698,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="30">
+    <row r="99" spans="1:5" ht="30" hidden="1">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>5</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30" hidden="1">
@@ -3463,7 +3463,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" hidden="1">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="30">
+    <row r="167" spans="1:5" ht="30" hidden="1">
       <c r="A167" s="2">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Solution for "103. Binary Tree Zigzag Level Order Traversal". zen-1
</commit_message>
<xml_diff>
--- a/meta/progress.xlsx
+++ b/meta/progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14900" yWindow="860" windowWidth="22960" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="6960" yWindow="0" windowWidth="19880" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
+      <selection pane="bottomLeft" activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2426,7 +2426,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="30">
+    <row r="83" spans="1:5" ht="30" hidden="1">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>5</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" hidden="1">
@@ -2783,7 +2783,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="30">
+    <row r="104" spans="1:5" ht="30" hidden="1">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>5</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30" hidden="1">

</xml_diff>

<commit_message>
Solution for "129. Sum Root to Leaf Numbers". zen-1
</commit_message>
<xml_diff>
--- a/meta/progress.xlsx
+++ b/meta/progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="0" windowWidth="19880" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="10440" yWindow="0" windowWidth="17220" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -637,12 +637,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -658,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -689,6 +695,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1026,7 +1035,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E107" sqref="E107"/>
+      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2817,7 +2826,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="45">
+    <row r="106" spans="1:5" ht="45" hidden="1">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2831,7 +2840,7 @@
         <v>5</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="45">
@@ -3089,7 +3098,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="30">
+    <row r="122" spans="1:5" ht="30" hidden="1">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -3103,10 +3112,10 @@
         <v>5</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="30">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="30" hidden="1">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -3120,7 +3129,7 @@
         <v>5</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="30" hidden="1">
@@ -3225,7 +3234,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="30">
+    <row r="130" spans="1:5" ht="30" hidden="1">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -3239,10 +3248,10 @@
         <v>5</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" hidden="1">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -3256,10 +3265,10 @@
         <v>5</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" hidden="1">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -3273,7 +3282,7 @@
         <v>5</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="30" hidden="1">
@@ -3684,7 +3693,7 @@
       <c r="A157" s="2">
         <v>156</v>
       </c>
-      <c r="B157" s="6" t="s">
+      <c r="B157" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C157" s="3">
@@ -3769,7 +3778,7 @@
       <c r="A162" s="2">
         <v>161</v>
       </c>
-      <c r="B162" s="6" t="s">
+      <c r="B162" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C162" s="3">
@@ -3803,7 +3812,7 @@
       <c r="A164" s="2">
         <v>163</v>
       </c>
-      <c r="B164" s="6" t="s">
+      <c r="B164" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C164" s="3">
@@ -3869,7 +3878,7 @@
       <c r="A168" s="2">
         <v>167</v>
       </c>
-      <c r="B168" s="6" t="s">
+      <c r="B168" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C168" s="3">
@@ -4022,7 +4031,7 @@
       <c r="A177" s="2">
         <v>186</v>
       </c>
-      <c r="B177" s="6" t="s">
+      <c r="B177" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C177" s="3">

</xml_diff>

<commit_message>
Solution for "116. Populating Next Right Pointers in Each Node". zen-1
</commit_message>
<xml_diff>
--- a/meta/progress.xlsx
+++ b/meta/progress.xlsx
@@ -1034,8 +1034,8 @@
   <dimension ref="A1:O184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3013,7 +3013,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="30">
+    <row r="117" spans="1:5" ht="30" hidden="1">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>5</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30" hidden="1">
@@ -3200,7 +3200,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" hidden="1">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>5</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30" hidden="1">

</xml_diff>